<commit_message>
added some issue6 data
</commit_message>
<xml_diff>
--- a/raincloudQuartet_R/dataPbrPlotting.xlsx
+++ b/raincloudQuartet_R/dataPbrPlotting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Documents/projects/raincloudQuartet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Documents/GitHub/raincloudQuartet/raincloudQuartet_R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74C096B-3F9C-1B43-889C-5BF5A6F0B555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBB56BE-77A6-D348-A30B-47889707F481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{3C382137-58E4-F94B-B043-CDE1DB9A046F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="402">
   <si>
     <t>firstAuthor</t>
   </si>
@@ -1188,6 +1188,60 @@
   </si>
   <si>
     <t>used general logistc linear models; some descriptives to these analyses could also have been plotted</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>Tracking the first two seconds: three stages of visual information processing?</t>
+  </si>
+  <si>
+    <t>Dimensional overlap between time and space</t>
+  </si>
+  <si>
+    <t>Eikmeier</t>
+  </si>
+  <si>
+    <t>The benefits and costs of comparisons in a novel object categorization task: Interactions with development</t>
+  </si>
+  <si>
+    <t>Augier</t>
+  </si>
+  <si>
+    <t>Manning</t>
+  </si>
+  <si>
+    <t>“Moving to the beat” improves timing perception</t>
+  </si>
+  <si>
+    <t>Bindemann</t>
+  </si>
+  <si>
+    <t>Face detection differs from categorization: Evidence from visual search in natural scenes</t>
+  </si>
+  <si>
+    <t>Chesney</t>
+  </si>
+  <si>
+    <t>Knowledge on the line: Manipulating beliefs about the magnitudes of symbolic numbers affects the linearity of line estimation tasks</t>
+  </si>
+  <si>
+    <t>Beck</t>
+  </si>
+  <si>
+    <t>A new illusion of height and width: taller people are perceived as thinner</t>
+  </si>
+  <si>
+    <t>Glicksohn</t>
+  </si>
+  <si>
+    <t>The role of cross-modal associations in statistical learning</t>
+  </si>
+  <si>
+    <t>Evans</t>
+  </si>
+  <si>
+    <t>The gist of the abnormal: Above-chance medical decision making in the blink of an eye</t>
   </si>
 </sst>
 </file>
@@ -1598,11 +1652,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2065784-6E08-3B41-935B-785814B2408A}">
-  <dimension ref="A1:M134"/>
+  <dimension ref="A1:M143"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M131" sqref="M131"/>
+    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M143" sqref="M143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6430,6 +6484,243 @@
         <v>33</v>
       </c>
     </row>
+    <row r="135" spans="1:13" ht="32">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="C135">
+        <v>2013</v>
+      </c>
+      <c r="E135">
+        <v>6</v>
+      </c>
+      <c r="G135" t="s">
+        <v>384</v>
+      </c>
+      <c r="H135" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="I135" t="s">
+        <v>13</v>
+      </c>
+      <c r="J135" t="s">
+        <v>13</v>
+      </c>
+      <c r="K135" t="s">
+        <v>32</v>
+      </c>
+      <c r="L135" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" ht="32">
+      <c r="C136">
+        <v>2013</v>
+      </c>
+      <c r="E136">
+        <v>6</v>
+      </c>
+      <c r="G136" t="s">
+        <v>387</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="I136" t="s">
+        <v>13</v>
+      </c>
+      <c r="J136" t="s">
+        <v>13</v>
+      </c>
+      <c r="K136" t="s">
+        <v>32</v>
+      </c>
+      <c r="L136" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" ht="32">
+      <c r="C137">
+        <v>2013</v>
+      </c>
+      <c r="E137">
+        <v>6</v>
+      </c>
+      <c r="G137" t="s">
+        <v>389</v>
+      </c>
+      <c r="H137" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="I137" t="s">
+        <v>13</v>
+      </c>
+      <c r="J137" t="s">
+        <v>13</v>
+      </c>
+      <c r="K137" t="s">
+        <v>32</v>
+      </c>
+      <c r="L137" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" ht="32">
+      <c r="C138">
+        <v>2013</v>
+      </c>
+      <c r="E138">
+        <v>6</v>
+      </c>
+      <c r="G138" t="s">
+        <v>390</v>
+      </c>
+      <c r="H138" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="I138" t="s">
+        <v>13</v>
+      </c>
+      <c r="J138" t="s">
+        <v>13</v>
+      </c>
+      <c r="K138" t="s">
+        <v>32</v>
+      </c>
+      <c r="L138" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" ht="32">
+      <c r="C139">
+        <v>2013</v>
+      </c>
+      <c r="E139">
+        <v>6</v>
+      </c>
+      <c r="G139" t="s">
+        <v>392</v>
+      </c>
+      <c r="H139" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="I139" t="s">
+        <v>13</v>
+      </c>
+      <c r="J139" t="s">
+        <v>19</v>
+      </c>
+      <c r="K139" t="s">
+        <v>13</v>
+      </c>
+      <c r="L139" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" ht="32">
+      <c r="C140">
+        <v>2013</v>
+      </c>
+      <c r="E140">
+        <v>6</v>
+      </c>
+      <c r="G140" t="s">
+        <v>394</v>
+      </c>
+      <c r="H140" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="I140" t="s">
+        <v>19</v>
+      </c>
+      <c r="J140" t="s">
+        <v>32</v>
+      </c>
+      <c r="K140" t="s">
+        <v>32</v>
+      </c>
+      <c r="L140" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" ht="32">
+      <c r="C141">
+        <v>2013</v>
+      </c>
+      <c r="E141">
+        <v>6</v>
+      </c>
+      <c r="G141" t="s">
+        <v>396</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="I141" t="s">
+        <v>13</v>
+      </c>
+      <c r="J141" t="s">
+        <v>13</v>
+      </c>
+      <c r="K141" t="s">
+        <v>32</v>
+      </c>
+      <c r="L141" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" ht="32">
+      <c r="C142">
+        <v>2013</v>
+      </c>
+      <c r="E142">
+        <v>6</v>
+      </c>
+      <c r="G142" t="s">
+        <v>398</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="I142" t="s">
+        <v>13</v>
+      </c>
+      <c r="J142" t="s">
+        <v>19</v>
+      </c>
+      <c r="K142" t="s">
+        <v>13</v>
+      </c>
+      <c r="L142" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" ht="32">
+      <c r="C143">
+        <v>2013</v>
+      </c>
+      <c r="E143">
+        <v>6</v>
+      </c>
+      <c r="G143" t="s">
+        <v>400</v>
+      </c>
+      <c r="H143" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="I143" t="s">
+        <v>13</v>
+      </c>
+      <c r="J143" t="s">
+        <v>13</v>
+      </c>
+      <c r="K143" t="s">
+        <v>32</v>
+      </c>
+      <c r="L143" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished 2013 data collection
</commit_message>
<xml_diff>
--- a/raincloudQuartet_R/dataPbrPlotting.xlsx
+++ b/raincloudQuartet_R/dataPbrPlotting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Documents/GitHub/raincloudQuartet/raincloudQuartet_R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBB56BE-77A6-D348-A30B-47889707F481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A4358D-3016-574A-A91D-36DB6B15F339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{3C382137-58E4-F94B-B043-CDE1DB9A046F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="628">
   <si>
     <t>firstAuthor</t>
   </si>
@@ -1242,13 +1242,716 @@
   </si>
   <si>
     <t>The gist of the abnormal: Above-chance medical decision making in the blink of an eye</t>
+  </si>
+  <si>
+    <t>Yang</t>
+  </si>
+  <si>
+    <t>The cognitive advantage for one’s own name is not simply familiarity: An eye-tracking study</t>
+  </si>
+  <si>
+    <t>Arend</t>
+  </si>
+  <si>
+    <t>Numerical-spatial representation affects spatial coding: binding errors across the numerical distance effect</t>
+  </si>
+  <si>
+    <t>Burnham</t>
+  </si>
+  <si>
+    <t>Response retrieval in a go/no-go priming-of-popout task</t>
+  </si>
+  <si>
+    <t>Chen</t>
+  </si>
+  <si>
+    <t>When the voluntary mind meets the irresistible event: Stimulus–response correspondence effects on task selection during voluntary task switching</t>
+  </si>
+  <si>
+    <t>Lost ability to automatize task performance in old age</t>
+  </si>
+  <si>
+    <t>Maquestiaux</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Attention is biased to near surfaces</t>
+  </si>
+  <si>
+    <t>Wilder</t>
+  </si>
+  <si>
+    <t>The persistent impact of incidental experience</t>
+  </si>
+  <si>
+    <t>Takarangi</t>
+  </si>
+  <si>
+    <t>Source confusion influences the effectiveness of the autobiographical IAT</t>
+  </si>
+  <si>
+    <t>Vaughn</t>
+  </si>
+  <si>
+    <t>Repeated retrieval practice and item difficulty: Does criterion learning eliminate item difficulty effects?</t>
+  </si>
+  <si>
+    <t>Urgolites</t>
+  </si>
+  <si>
+    <t>Binding actions and scenes in visual long-term memory</t>
+  </si>
+  <si>
+    <t>Cowan</t>
+  </si>
+  <si>
+    <t>A list-length constraint on incidental item-to-item associations</t>
+  </si>
+  <si>
+    <t>Kang</t>
+  </si>
+  <si>
+    <t>Don’t just repeat after me: Retrieval practice is better than imitation for foreign vocabulary learning</t>
+  </si>
+  <si>
+    <t>Horn</t>
+  </si>
+  <si>
+    <t>Adult age differences in interference from a prospective-memory task: a diffusion model analysis</t>
+  </si>
+  <si>
+    <t>Minear</t>
+  </si>
+  <si>
+    <t>Working memory, fluid intelligence, and impulsiveness in heavy media multitaskers</t>
+  </si>
+  <si>
+    <t>Peterson</t>
+  </si>
+  <si>
+    <t>The Gestalt principle of similarity benefits visual working memory</t>
+  </si>
+  <si>
+    <t>Blalock</t>
+  </si>
+  <si>
+    <t>Mask similarity impacts short-term consolidation in visual working memory</t>
+  </si>
+  <si>
+    <t>Francis</t>
+  </si>
+  <si>
+    <t>The bilingual L2 advantage in recognition memory</t>
+  </si>
+  <si>
+    <t>Staub</t>
+  </si>
+  <si>
+    <t>Individual differences in fixation duration distributions in reading</t>
+  </si>
+  <si>
+    <t>Grasping the invisible: Semantic processing of abstract words</t>
+  </si>
+  <si>
+    <t>Zdrazilova</t>
+  </si>
+  <si>
+    <t>Barnhart</t>
+  </si>
+  <si>
+    <t>Rotation reveals the importance of configural cues in handwritten word perception</t>
+  </si>
+  <si>
+    <t>Shtulman</t>
+  </si>
+  <si>
+    <t>Cognitive parallels between moral judgment and modal judgment</t>
+  </si>
+  <si>
+    <t>Hochman</t>
+  </si>
+  <si>
+    <t>The partial-reinforcement extinction effect and the contingent-sampling hypothesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> there are plots, but the tables are what would actually correspond with a raincloud plot visualization</t>
+  </si>
+  <si>
+    <t>Tam</t>
+  </si>
+  <si>
+    <t>Posterror slowing predicts rule-based but not information-integration category learning</t>
+  </si>
+  <si>
+    <t>Carpenter</t>
+  </si>
+  <si>
+    <t>Appearances can be deceiving: instructor fluency increases perceptions of learning without increasing actual learning</t>
+  </si>
+  <si>
+    <t>Ikeda</t>
+  </si>
+  <si>
+    <t>Neuroscientific information bias in metacomprehension: The effect of brain images on metacomprehension judgment of neuroscience research</t>
+  </si>
+  <si>
+    <t>Witt</t>
+  </si>
+  <si>
+    <t>Catching ease influences perceived speed: Evidence for action-specific effects from action-based measures</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Multimodally specified energy expenditure and action-based distance judgments</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Color preferences in infants and adults are different</t>
+  </si>
+  <si>
+    <t>Shaffer</t>
+  </si>
+  <si>
+    <t>Blind(fold)ed by science: A constant target-heading angle is used in visual and nonvisual pursuit</t>
+  </si>
+  <si>
+    <t>Strauss</t>
+  </si>
+  <si>
+    <t>Color preferences change after experience with liked/disliked colored objects</t>
+  </si>
+  <si>
+    <t>Du</t>
+  </si>
+  <si>
+    <t>On the automaticity of contingent capture: disruption caused by the attentional blink</t>
+  </si>
+  <si>
+    <t>Ericson</t>
+  </si>
+  <si>
+    <t>Changing target trajectories influences tracking performance</t>
+  </si>
+  <si>
+    <t>Coelho</t>
+  </si>
+  <si>
+    <t>Is handedness just response bias?</t>
+  </si>
+  <si>
+    <t>Lagrou</t>
+  </si>
+  <si>
+    <t>Interlingual lexical competition in a spoken sentence context: Evidence from the visual world paradigm</t>
+  </si>
+  <si>
+    <t>Cai</t>
+  </si>
+  <si>
+    <t>Time does not flow without language: Spatial distance affects temporal duration regardless of movement or direction</t>
+  </si>
+  <si>
+    <t>Toscano</t>
+  </si>
+  <si>
+    <t>Reconsidering the role of temporal order in spoken word recognition</t>
+  </si>
+  <si>
+    <t>Letter transpositions within and across morphemic boundaries: Is there a cross-language difference?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sánchez-Gutiérrez </t>
+  </si>
+  <si>
+    <t>Stagner</t>
+  </si>
+  <si>
+    <t>The Monty Hall dilemma in pigeons: Effect of investment in initial choice</t>
+  </si>
+  <si>
+    <t>Halvorson</t>
+  </si>
+  <si>
+    <t>Conceptualization of task boundaries preserves implicit sequence learning under dual-task conditions</t>
+  </si>
+  <si>
+    <t>Colzato</t>
+  </si>
+  <si>
+    <t>Increasing self–other integration through divergent thinking</t>
+  </si>
+  <si>
+    <t>Moxley</t>
+  </si>
+  <si>
+    <t>Meta-analysis of age and skill effects on recalling chess positions and selecting the best move</t>
+  </si>
+  <si>
+    <t>Hills</t>
+  </si>
+  <si>
+    <t>Information overload or search-amplified risk? Set size and order effects on decisions from experience</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>On the (non)persuasive power of a brain image</t>
+  </si>
+  <si>
+    <t>Kangas</t>
+  </si>
+  <si>
+    <t>Parts function as perceptual organizational entities in infancy</t>
+  </si>
+  <si>
+    <t>Pinto</t>
+  </si>
+  <si>
+    <t>Fragile visual short-term memory is an object-based and location-specific store</t>
+  </si>
+  <si>
+    <t>Sherman</t>
+  </si>
+  <si>
+    <t>Auditory rhythms are systemically associated with spatial-frequency and density information in visual scenes</t>
+  </si>
+  <si>
+    <t>Pfordresher</t>
+  </si>
+  <si>
+    <t>Auditory imagery and the poor-pitch singer</t>
+  </si>
+  <si>
+    <t>Stevenson</t>
+  </si>
+  <si>
+    <t>Familiarity influences odor memory stability</t>
+  </si>
+  <si>
+    <t>chi square test</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Both young and older adults discount suggestions from older adults on a social memory test</t>
+  </si>
+  <si>
+    <t>Wardlow</t>
+  </si>
+  <si>
+    <t>Individual differences in speakers’ perspective taking: The roles of executive control and working memory</t>
+  </si>
+  <si>
+    <t>Li</t>
+  </si>
+  <si>
+    <t>The activation of segmental and tonal information in visual word recognition</t>
+  </si>
+  <si>
+    <t>Finley</t>
+  </si>
+  <si>
+    <t>Generalization to unfamiliar talkers in artificial language learning</t>
+  </si>
+  <si>
+    <t>Hattori</t>
+  </si>
+  <si>
+    <t>Effects of subliminal hints on insight problem solving</t>
+  </si>
+  <si>
+    <t>Duthoo</t>
+  </si>
+  <si>
+    <t>The hot-hand fallacy in cognitive control: Repetition expectancy modulates the congruency sequence effect</t>
+  </si>
+  <si>
+    <t>Pennycook</t>
+  </si>
+  <si>
+    <t>Belief bias during reasoning among religious believers and skeptics</t>
+  </si>
+  <si>
+    <t>Wright</t>
+  </si>
+  <si>
+    <t>Delay and déjà vu: Timing and repetition increase the power of false evidence</t>
+  </si>
+  <si>
+    <t>Palmer</t>
+  </si>
+  <si>
+    <t>Accounting for taste: Individual differences in preference for harmony</t>
+  </si>
+  <si>
+    <t>Morgado</t>
+  </si>
+  <si>
+    <t>Within reach but not so reachable: Obstacles matter in visual perception of distances</t>
+  </si>
+  <si>
+    <t>de Fockert</t>
+  </si>
+  <si>
+    <t>Greater visual averaging of face identity for own-gender faces</t>
+  </si>
+  <si>
+    <t>Fiedler</t>
+  </si>
+  <si>
+    <t>Redundancy gain for semantic features</t>
+  </si>
+  <si>
+    <t>Liefooghe</t>
+  </si>
+  <si>
+    <t>Instruction-based response activation depends on task preparation</t>
+  </si>
+  <si>
+    <t>Carneiro</t>
+  </si>
+  <si>
+    <t>Retrieval dynamics in false recall: revelations from identifiability manipulations</t>
+  </si>
+  <si>
+    <t>Marstaller</t>
+  </si>
+  <si>
+    <t>Individual differences in the gesture effect on working memory</t>
+  </si>
+  <si>
+    <t>Fenn</t>
+  </si>
+  <si>
+    <t>What drives sleep-dependent memory consolidation: Greater gain or less loss?</t>
+  </si>
+  <si>
+    <t>Arnold</t>
+  </si>
+  <si>
+    <t>Free recall enhances subsequent learning</t>
+  </si>
+  <si>
+    <t>The boundary conditions of priming of visual search: From passive viewing through task-relevant working memory load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kristjánsson </t>
+  </si>
+  <si>
+    <t>Bugg</t>
+  </si>
+  <si>
+    <t>Strengthening encoding via implementation intention formation increases prospective memory commission errors</t>
+  </si>
+  <si>
+    <t>Brinegar</t>
+  </si>
+  <si>
+    <t>Improving memory after environmental context change: A strategy of “preinstatement”</t>
+  </si>
+  <si>
+    <t>Marelli</t>
+  </si>
+  <si>
+    <t>Meaning is in the beholder’s eye: Morpho-semantic effects in masked priming</t>
+  </si>
+  <si>
+    <t>Connell</t>
+  </si>
+  <si>
+    <t>Flexible and fast: Linguistic shortcut affects both shallow and deep conceptual processing</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>What’s left? An eye movement study of the influence of interword spaces to the left of fixation during reading</t>
+  </si>
+  <si>
+    <t>Hewitt</t>
+  </si>
+  <si>
+    <t>Speaking order predicts memory conformity after accounting for exposure to misinformation</t>
+  </si>
+  <si>
+    <t>Sanders</t>
+  </si>
+  <si>
+    <t>Is better beautiful or is beautiful better? Exploring the relationship between beauty and category structure</t>
+  </si>
+  <si>
+    <t>Cyr</t>
+  </si>
+  <si>
+    <t>Updating misconceptions: Effects of age and confidence</t>
+  </si>
+  <si>
+    <t>Zabelina</t>
+  </si>
+  <si>
+    <t>Suppressed semantic information accelerates analytic problem solving</t>
+  </si>
+  <si>
+    <t>Feng</t>
+  </si>
+  <si>
+    <t>Mind wandering while reading easy and difficult texts</t>
+  </si>
+  <si>
+    <t>Hilchey</t>
+  </si>
+  <si>
+    <t>On the nature of the delayed “inhibitory” Cueing effects generated by uninformative arrows at fixation</t>
+  </si>
+  <si>
+    <t>anova in appendix with table, but not central to study if in appendix</t>
+  </si>
+  <si>
+    <t>Simons</t>
+  </si>
+  <si>
+    <t>Unskilled and optimistic: Overconfident predictions despite calibrated knowledge of relative skill</t>
+  </si>
+  <si>
+    <t>Rusou</t>
+  </si>
+  <si>
+    <t>Pitting intuitive and analytical thinking against each other: The case of transitivity</t>
+  </si>
+  <si>
+    <t>De Neys</t>
+  </si>
+  <si>
+    <t>Bats, balls, and substitution sensitivity: cognitive misers are no happy fools</t>
+  </si>
+  <si>
+    <t>Sanocki</t>
+  </si>
+  <si>
+    <t>Facilitatory priming of scene layout depends on experience with the scene</t>
+  </si>
+  <si>
+    <t>Jiang</t>
+  </si>
+  <si>
+    <t>The time course of attentional deployment in contextual cueing</t>
+  </si>
+  <si>
+    <t>Badham</t>
+  </si>
+  <si>
+    <t>Replicating distinctive facial features in lineups: identification performance in young versus older adults</t>
+  </si>
+  <si>
+    <t>Sawaki</t>
+  </si>
+  <si>
+    <t>Active suppression after involuntary capture of attention</t>
+  </si>
+  <si>
+    <t>Young</t>
+  </si>
+  <si>
+    <t>Magnitude effects for experienced rewards at short delays in the escalating interest task</t>
+  </si>
+  <si>
+    <t>Challenging prior evidence for a shared syntactic processor for language and music</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perruchet </t>
+  </si>
+  <si>
+    <t>Harlow</t>
+  </si>
+  <si>
+    <t>Source accuracy data reveal the thresholded nature of human episodic memory</t>
+  </si>
+  <si>
+    <t>Hierarchical modeling of contingency-based source monitoring: A test of the probability-matching account</t>
+  </si>
+  <si>
+    <t>Weywadt</t>
+  </si>
+  <si>
+    <t>The role of verbal short-term memory in task selection: How articulatory suppression influences task choice in voluntary task switching</t>
+  </si>
+  <si>
+    <t>Bui</t>
+  </si>
+  <si>
+    <t>The roles of working memory and intervening task difficulty in determining the benefits of repetition</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>The benefit of forgetting</t>
+  </si>
+  <si>
+    <t>Tauber</t>
+  </si>
+  <si>
+    <t>Self-regulated learning of a natural category: Do people interleave or block exemplars during study?</t>
+  </si>
+  <si>
+    <t>Worthy</t>
+  </si>
+  <si>
+    <t>Heterogeneity of strategy use in the Iowa gambling task: A comparison of win-stay/lose-shift and reinforcement learning models</t>
+  </si>
+  <si>
+    <t>Khader</t>
+  </si>
+  <si>
+    <t>Automatic activation of attribute knowledge in heuristic inference from memory</t>
+  </si>
+  <si>
+    <t>Mueller</t>
+  </si>
+  <si>
+    <t>Contributions of beliefs and processing fluency to the effect of relatedness on judgments of learning</t>
+  </si>
+  <si>
+    <t>Molet</t>
+  </si>
+  <si>
+    <t>Guilt by association and honor by association: The role of acquired equivalence</t>
+  </si>
+  <si>
+    <t>Ferguson</t>
+  </si>
+  <si>
+    <t>Examining mental simulations of uncertain events</t>
+  </si>
+  <si>
+    <t>Rey</t>
+  </si>
+  <si>
+    <t>The unbearable articulatory nature of naming: on the reliability of word naming responses at the item level</t>
+  </si>
+  <si>
+    <t>Mirror image arm used in monocular, binocular, and blindfolded pointing</t>
+  </si>
+  <si>
+    <t>Wnuczko</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Interacting with objects compresses environmental representations in spatial memory</t>
+  </si>
+  <si>
+    <t>Iordanescu</t>
+  </si>
+  <si>
+    <t>Action enhances auditory but not visual temporal sensitivity</t>
+  </si>
+  <si>
+    <t>Tye-Murray</t>
+  </si>
+  <si>
+    <t>Reading your own lips: Common-coding theory and visual speech perception</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Attention improves perceptual quality</t>
+  </si>
+  <si>
+    <t>Irwin</t>
+  </si>
+  <si>
+    <t>Visual marking across eye blinks</t>
+  </si>
+  <si>
+    <t>Dual n-back training increases the capacity of the focus of attention</t>
+  </si>
+  <si>
+    <t>Lilienthal</t>
+  </si>
+  <si>
+    <t>Hoch</t>
+  </si>
+  <si>
+    <t>Regularity of unit length boosts statistical learning in verbal and nonverbal artificial languages</t>
+  </si>
+  <si>
+    <t>Navarrete</t>
+  </si>
+  <si>
+    <t>Age-of-acquisition effects in delayed picture-naming tasks</t>
+  </si>
+  <si>
+    <t>The syllable as the proximate unit in Mandarin Chinese word production: An intrinsic or accidental property of the production system?</t>
+  </si>
+  <si>
+    <t>Morey</t>
+  </si>
+  <si>
+    <t>Visual short-term memory always requires general attention</t>
+  </si>
+  <si>
+    <t>yees</t>
+  </si>
+  <si>
+    <t>Lange</t>
+  </si>
+  <si>
+    <t>Working memory dynamics bias the generation of beliefs: The influence of data presentation rate on hypothesis generation</t>
+  </si>
+  <si>
+    <t>Chauvel</t>
+  </si>
+  <si>
+    <t>Novice motor performance: Better not to verbalize</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Negative prospective memory: Remembering </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to perform an action</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1289,6 +1992,20 @@
       <color theme="1"/>
       <name val="MyriadPro"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF111111"/>
+      <name val="AdvTTb8864ccf.B"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1310,7 +2027,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1318,6 +2035,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1652,11 +2370,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2065784-6E08-3B41-935B-785814B2408A}">
-  <dimension ref="A1:M143"/>
+  <dimension ref="A1:M255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M143" sqref="M143"/>
+      <pane ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F256" sqref="F256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6488,6 +7206,9 @@
       <c r="A135">
         <v>134</v>
       </c>
+      <c r="B135" t="s">
+        <v>10</v>
+      </c>
       <c r="C135">
         <v>2013</v>
       </c>
@@ -6514,6 +7235,12 @@
       </c>
     </row>
     <row r="136" spans="1:13" ht="32">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>10</v>
+      </c>
       <c r="C136">
         <v>2013</v>
       </c>
@@ -6540,6 +7267,12 @@
       </c>
     </row>
     <row r="137" spans="1:13" ht="32">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>10</v>
+      </c>
       <c r="C137">
         <v>2013</v>
       </c>
@@ -6566,6 +7299,12 @@
       </c>
     </row>
     <row r="138" spans="1:13" ht="32">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>10</v>
+      </c>
       <c r="C138">
         <v>2013</v>
       </c>
@@ -6592,6 +7331,12 @@
       </c>
     </row>
     <row r="139" spans="1:13" ht="32">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>10</v>
+      </c>
       <c r="C139">
         <v>2013</v>
       </c>
@@ -6618,6 +7363,12 @@
       </c>
     </row>
     <row r="140" spans="1:13" ht="32">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>10</v>
+      </c>
       <c r="C140">
         <v>2013</v>
       </c>
@@ -6644,6 +7395,12 @@
       </c>
     </row>
     <row r="141" spans="1:13" ht="32">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>10</v>
+      </c>
       <c r="C141">
         <v>2013</v>
       </c>
@@ -6670,6 +7427,12 @@
       </c>
     </row>
     <row r="142" spans="1:13" ht="32">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>10</v>
+      </c>
       <c r="C142">
         <v>2013</v>
       </c>
@@ -6696,6 +7459,12 @@
       </c>
     </row>
     <row r="143" spans="1:13" ht="32">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>10</v>
+      </c>
       <c r="C143">
         <v>2013</v>
       </c>
@@ -6719,6 +7488,3599 @@
       </c>
       <c r="L143" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" ht="32">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144">
+        <v>2013</v>
+      </c>
+      <c r="E144">
+        <v>6</v>
+      </c>
+      <c r="G144" t="s">
+        <v>402</v>
+      </c>
+      <c r="H144" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="I144" t="s">
+        <v>13</v>
+      </c>
+      <c r="J144" t="s">
+        <v>19</v>
+      </c>
+      <c r="K144" t="s">
+        <v>13</v>
+      </c>
+      <c r="L144" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" ht="32">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>10</v>
+      </c>
+      <c r="C145">
+        <v>2013</v>
+      </c>
+      <c r="E145">
+        <v>6</v>
+      </c>
+      <c r="G145" t="s">
+        <v>404</v>
+      </c>
+      <c r="H145" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="I145" t="s">
+        <v>13</v>
+      </c>
+      <c r="J145" t="s">
+        <v>13</v>
+      </c>
+      <c r="K145" t="s">
+        <v>32</v>
+      </c>
+      <c r="L145" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" ht="32">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
+        <v>10</v>
+      </c>
+      <c r="C146">
+        <v>2013</v>
+      </c>
+      <c r="E146">
+        <v>6</v>
+      </c>
+      <c r="G146" t="s">
+        <v>406</v>
+      </c>
+      <c r="H146" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="I146" t="s">
+        <v>13</v>
+      </c>
+      <c r="J146" t="s">
+        <v>13</v>
+      </c>
+      <c r="K146" t="s">
+        <v>32</v>
+      </c>
+      <c r="L146" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" ht="32">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>10</v>
+      </c>
+      <c r="C147">
+        <v>2013</v>
+      </c>
+      <c r="E147">
+        <v>6</v>
+      </c>
+      <c r="G147" t="s">
+        <v>408</v>
+      </c>
+      <c r="H147" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="I147" t="s">
+        <v>13</v>
+      </c>
+      <c r="J147" t="s">
+        <v>13</v>
+      </c>
+      <c r="K147" t="s">
+        <v>32</v>
+      </c>
+      <c r="L147" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" ht="32">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>10</v>
+      </c>
+      <c r="C148">
+        <v>2013</v>
+      </c>
+      <c r="E148">
+        <v>6</v>
+      </c>
+      <c r="G148" t="s">
+        <v>411</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="I148" t="s">
+        <v>13</v>
+      </c>
+      <c r="J148" t="s">
+        <v>13</v>
+      </c>
+      <c r="K148" t="s">
+        <v>32</v>
+      </c>
+      <c r="L148" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" ht="32">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
+        <v>10</v>
+      </c>
+      <c r="C149">
+        <v>2013</v>
+      </c>
+      <c r="E149">
+        <v>6</v>
+      </c>
+      <c r="G149" t="s">
+        <v>412</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="I149" t="s">
+        <v>19</v>
+      </c>
+      <c r="J149" t="s">
+        <v>32</v>
+      </c>
+      <c r="K149" t="s">
+        <v>32</v>
+      </c>
+      <c r="L149" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" ht="32">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
+        <v>10</v>
+      </c>
+      <c r="C150">
+        <v>2013</v>
+      </c>
+      <c r="E150">
+        <v>6</v>
+      </c>
+      <c r="G150" t="s">
+        <v>414</v>
+      </c>
+      <c r="H150" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="I150" t="s">
+        <v>13</v>
+      </c>
+      <c r="J150" t="s">
+        <v>13</v>
+      </c>
+      <c r="K150" t="s">
+        <v>32</v>
+      </c>
+      <c r="L150" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" ht="32">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>10</v>
+      </c>
+      <c r="C151">
+        <v>2013</v>
+      </c>
+      <c r="E151">
+        <v>6</v>
+      </c>
+      <c r="G151" t="s">
+        <v>416</v>
+      </c>
+      <c r="H151" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="I151" t="s">
+        <v>13</v>
+      </c>
+      <c r="J151" t="s">
+        <v>13</v>
+      </c>
+      <c r="K151" t="s">
+        <v>32</v>
+      </c>
+      <c r="L151" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" ht="32">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>10</v>
+      </c>
+      <c r="C152">
+        <v>2013</v>
+      </c>
+      <c r="E152">
+        <v>6</v>
+      </c>
+      <c r="G152" t="s">
+        <v>418</v>
+      </c>
+      <c r="H152" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="I152" t="s">
+        <v>13</v>
+      </c>
+      <c r="J152" t="s">
+        <v>13</v>
+      </c>
+      <c r="K152" t="s">
+        <v>32</v>
+      </c>
+      <c r="L152" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" ht="32">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>10</v>
+      </c>
+      <c r="C153">
+        <v>2013</v>
+      </c>
+      <c r="E153">
+        <v>6</v>
+      </c>
+      <c r="G153" t="s">
+        <v>420</v>
+      </c>
+      <c r="H153" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="I153" t="s">
+        <v>13</v>
+      </c>
+      <c r="J153" t="s">
+        <v>13</v>
+      </c>
+      <c r="K153" t="s">
+        <v>32</v>
+      </c>
+      <c r="L153" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" ht="32">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>10</v>
+      </c>
+      <c r="C154">
+        <v>2013</v>
+      </c>
+      <c r="E154">
+        <v>6</v>
+      </c>
+      <c r="G154" t="s">
+        <v>422</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="I154" t="s">
+        <v>13</v>
+      </c>
+      <c r="J154" t="s">
+        <v>13</v>
+      </c>
+      <c r="K154" t="s">
+        <v>32</v>
+      </c>
+      <c r="L154" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" ht="32">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>10</v>
+      </c>
+      <c r="C155">
+        <v>2013</v>
+      </c>
+      <c r="E155">
+        <v>6</v>
+      </c>
+      <c r="G155" t="s">
+        <v>424</v>
+      </c>
+      <c r="H155" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="I155" t="s">
+        <v>13</v>
+      </c>
+      <c r="J155" t="s">
+        <v>13</v>
+      </c>
+      <c r="K155" t="s">
+        <v>32</v>
+      </c>
+      <c r="L155" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" ht="32">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
+        <v>10</v>
+      </c>
+      <c r="C156">
+        <v>2013</v>
+      </c>
+      <c r="E156">
+        <v>6</v>
+      </c>
+      <c r="G156" t="s">
+        <v>426</v>
+      </c>
+      <c r="H156" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="I156" t="s">
+        <v>13</v>
+      </c>
+      <c r="J156" t="s">
+        <v>13</v>
+      </c>
+      <c r="K156" t="s">
+        <v>32</v>
+      </c>
+      <c r="L156" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" ht="32">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
+        <v>10</v>
+      </c>
+      <c r="C157">
+        <v>2013</v>
+      </c>
+      <c r="E157">
+        <v>6</v>
+      </c>
+      <c r="G157" t="s">
+        <v>428</v>
+      </c>
+      <c r="H157" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="I157" t="s">
+        <v>13</v>
+      </c>
+      <c r="J157" t="s">
+        <v>13</v>
+      </c>
+      <c r="K157" t="s">
+        <v>32</v>
+      </c>
+      <c r="L157" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" ht="32">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158">
+        <v>2013</v>
+      </c>
+      <c r="E158">
+        <v>6</v>
+      </c>
+      <c r="G158" t="s">
+        <v>430</v>
+      </c>
+      <c r="H158" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="I158" t="s">
+        <v>13</v>
+      </c>
+      <c r="J158" t="s">
+        <v>13</v>
+      </c>
+      <c r="K158" t="s">
+        <v>32</v>
+      </c>
+      <c r="L158" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" ht="32">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" t="s">
+        <v>10</v>
+      </c>
+      <c r="C159">
+        <v>2013</v>
+      </c>
+      <c r="E159">
+        <v>6</v>
+      </c>
+      <c r="G159" t="s">
+        <v>432</v>
+      </c>
+      <c r="H159" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I159" t="s">
+        <v>13</v>
+      </c>
+      <c r="J159" t="s">
+        <v>13</v>
+      </c>
+      <c r="K159" t="s">
+        <v>32</v>
+      </c>
+      <c r="L159" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" ht="32">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" t="s">
+        <v>10</v>
+      </c>
+      <c r="C160">
+        <v>2013</v>
+      </c>
+      <c r="E160">
+        <v>6</v>
+      </c>
+      <c r="G160" t="s">
+        <v>434</v>
+      </c>
+      <c r="H160" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="I160" t="s">
+        <v>13</v>
+      </c>
+      <c r="J160" t="s">
+        <v>13</v>
+      </c>
+      <c r="K160" t="s">
+        <v>32</v>
+      </c>
+      <c r="L160" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" ht="32">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" t="s">
+        <v>10</v>
+      </c>
+      <c r="C161">
+        <v>2013</v>
+      </c>
+      <c r="E161">
+        <v>6</v>
+      </c>
+      <c r="G161" t="s">
+        <v>436</v>
+      </c>
+      <c r="H161" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="I161" t="s">
+        <v>19</v>
+      </c>
+      <c r="J161" t="s">
+        <v>32</v>
+      </c>
+      <c r="K161" t="s">
+        <v>32</v>
+      </c>
+      <c r="L161" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" ht="32">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" t="s">
+        <v>10</v>
+      </c>
+      <c r="C162">
+        <v>2013</v>
+      </c>
+      <c r="E162">
+        <v>6</v>
+      </c>
+      <c r="G162" t="s">
+        <v>439</v>
+      </c>
+      <c r="H162" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="I162" t="s">
+        <v>19</v>
+      </c>
+      <c r="J162" t="s">
+        <v>32</v>
+      </c>
+      <c r="K162" t="s">
+        <v>32</v>
+      </c>
+      <c r="L162" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" ht="32">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" t="s">
+        <v>10</v>
+      </c>
+      <c r="C163">
+        <v>2013</v>
+      </c>
+      <c r="E163">
+        <v>6</v>
+      </c>
+      <c r="G163" t="s">
+        <v>440</v>
+      </c>
+      <c r="H163" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="I163" t="s">
+        <v>13</v>
+      </c>
+      <c r="J163" t="s">
+        <v>13</v>
+      </c>
+      <c r="K163" t="s">
+        <v>32</v>
+      </c>
+      <c r="L163" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" ht="32">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" t="s">
+        <v>10</v>
+      </c>
+      <c r="C164">
+        <v>2013</v>
+      </c>
+      <c r="E164">
+        <v>6</v>
+      </c>
+      <c r="G164" t="s">
+        <v>442</v>
+      </c>
+      <c r="H164" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="I164" t="s">
+        <v>13</v>
+      </c>
+      <c r="J164" t="s">
+        <v>13</v>
+      </c>
+      <c r="K164" t="s">
+        <v>32</v>
+      </c>
+      <c r="L164" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" ht="32">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165" t="s">
+        <v>10</v>
+      </c>
+      <c r="C165">
+        <v>2013</v>
+      </c>
+      <c r="E165">
+        <v>6</v>
+      </c>
+      <c r="G165" t="s">
+        <v>444</v>
+      </c>
+      <c r="H165" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="I165" t="s">
+        <v>13</v>
+      </c>
+      <c r="J165" t="s">
+        <v>19</v>
+      </c>
+      <c r="K165" t="s">
+        <v>13</v>
+      </c>
+      <c r="L165" t="s">
+        <v>73</v>
+      </c>
+      <c r="M165" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" ht="32">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166" t="s">
+        <v>10</v>
+      </c>
+      <c r="C166">
+        <v>2013</v>
+      </c>
+      <c r="E166">
+        <v>6</v>
+      </c>
+      <c r="G166" t="s">
+        <v>447</v>
+      </c>
+      <c r="H166" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="I166" t="s">
+        <v>13</v>
+      </c>
+      <c r="J166" t="s">
+        <v>13</v>
+      </c>
+      <c r="K166" t="s">
+        <v>32</v>
+      </c>
+      <c r="L166" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" ht="32">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" t="s">
+        <v>10</v>
+      </c>
+      <c r="C167">
+        <v>2013</v>
+      </c>
+      <c r="E167">
+        <v>6</v>
+      </c>
+      <c r="G167" t="s">
+        <v>449</v>
+      </c>
+      <c r="H167" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="I167" t="s">
+        <v>13</v>
+      </c>
+      <c r="J167" t="s">
+        <v>13</v>
+      </c>
+      <c r="K167" t="s">
+        <v>32</v>
+      </c>
+      <c r="L167" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" ht="32">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" t="s">
+        <v>10</v>
+      </c>
+      <c r="C168">
+        <v>2013</v>
+      </c>
+      <c r="E168">
+        <v>6</v>
+      </c>
+      <c r="G168" t="s">
+        <v>451</v>
+      </c>
+      <c r="H168" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="I168" t="s">
+        <v>13</v>
+      </c>
+      <c r="J168" t="s">
+        <v>13</v>
+      </c>
+      <c r="K168" t="s">
+        <v>32</v>
+      </c>
+      <c r="L168" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" ht="32">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" t="s">
+        <v>10</v>
+      </c>
+      <c r="C169">
+        <v>2013</v>
+      </c>
+      <c r="E169">
+        <v>6</v>
+      </c>
+      <c r="G169" t="s">
+        <v>453</v>
+      </c>
+      <c r="H169" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="I169" t="s">
+        <v>13</v>
+      </c>
+      <c r="J169" t="s">
+        <v>13</v>
+      </c>
+      <c r="K169" t="s">
+        <v>32</v>
+      </c>
+      <c r="L169" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" ht="32">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" t="s">
+        <v>10</v>
+      </c>
+      <c r="C170">
+        <v>2013</v>
+      </c>
+      <c r="E170">
+        <v>6</v>
+      </c>
+      <c r="G170" t="s">
+        <v>455</v>
+      </c>
+      <c r="H170" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="I170" t="s">
+        <v>13</v>
+      </c>
+      <c r="J170" t="s">
+        <v>13</v>
+      </c>
+      <c r="K170" t="s">
+        <v>32</v>
+      </c>
+      <c r="L170" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" ht="32">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171" t="s">
+        <v>10</v>
+      </c>
+      <c r="C171">
+        <v>2013</v>
+      </c>
+      <c r="E171">
+        <v>5</v>
+      </c>
+      <c r="G171" t="s">
+        <v>457</v>
+      </c>
+      <c r="H171" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="I171" t="s">
+        <v>13</v>
+      </c>
+      <c r="J171" t="s">
+        <v>13</v>
+      </c>
+      <c r="K171" t="s">
+        <v>32</v>
+      </c>
+      <c r="L171" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" ht="32">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
+        <v>10</v>
+      </c>
+      <c r="C172">
+        <v>2013</v>
+      </c>
+      <c r="E172">
+        <v>5</v>
+      </c>
+      <c r="G172" t="s">
+        <v>459</v>
+      </c>
+      <c r="H172" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="I172" t="s">
+        <v>13</v>
+      </c>
+      <c r="J172" t="s">
+        <v>19</v>
+      </c>
+      <c r="K172" t="s">
+        <v>19</v>
+      </c>
+      <c r="L172" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" ht="32">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" t="s">
+        <v>10</v>
+      </c>
+      <c r="C173">
+        <v>2013</v>
+      </c>
+      <c r="E173">
+        <v>5</v>
+      </c>
+      <c r="G173" t="s">
+        <v>461</v>
+      </c>
+      <c r="H173" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="I173" t="s">
+        <v>13</v>
+      </c>
+      <c r="J173" t="s">
+        <v>13</v>
+      </c>
+      <c r="K173" t="s">
+        <v>32</v>
+      </c>
+      <c r="L173" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" ht="32">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" t="s">
+        <v>10</v>
+      </c>
+      <c r="C174">
+        <v>2013</v>
+      </c>
+      <c r="E174">
+        <v>5</v>
+      </c>
+      <c r="G174" t="s">
+        <v>463</v>
+      </c>
+      <c r="H174" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="I174" t="s">
+        <v>13</v>
+      </c>
+      <c r="J174" t="s">
+        <v>13</v>
+      </c>
+      <c r="K174" t="s">
+        <v>32</v>
+      </c>
+      <c r="L174" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" ht="32">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175" t="s">
+        <v>10</v>
+      </c>
+      <c r="C175">
+        <v>2013</v>
+      </c>
+      <c r="E175">
+        <v>5</v>
+      </c>
+      <c r="G175" t="s">
+        <v>465</v>
+      </c>
+      <c r="H175" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I175" t="s">
+        <v>13</v>
+      </c>
+      <c r="J175" t="s">
+        <v>13</v>
+      </c>
+      <c r="K175" t="s">
+        <v>32</v>
+      </c>
+      <c r="L175" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" ht="32">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176" t="s">
+        <v>10</v>
+      </c>
+      <c r="C176">
+        <v>2013</v>
+      </c>
+      <c r="E176">
+        <v>5</v>
+      </c>
+      <c r="G176" t="s">
+        <v>467</v>
+      </c>
+      <c r="H176" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="I176" t="s">
+        <v>13</v>
+      </c>
+      <c r="J176" t="s">
+        <v>13</v>
+      </c>
+      <c r="K176" t="s">
+        <v>32</v>
+      </c>
+      <c r="L176" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" ht="32">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177" t="s">
+        <v>10</v>
+      </c>
+      <c r="C177">
+        <v>2013</v>
+      </c>
+      <c r="E177">
+        <v>5</v>
+      </c>
+      <c r="G177" t="s">
+        <v>469</v>
+      </c>
+      <c r="H177" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="I177" t="s">
+        <v>13</v>
+      </c>
+      <c r="J177" t="s">
+        <v>13</v>
+      </c>
+      <c r="K177" t="s">
+        <v>32</v>
+      </c>
+      <c r="L177" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" ht="32">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178" t="s">
+        <v>10</v>
+      </c>
+      <c r="C178">
+        <v>2013</v>
+      </c>
+      <c r="E178">
+        <v>5</v>
+      </c>
+      <c r="G178" t="s">
+        <v>471</v>
+      </c>
+      <c r="H178" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="I178" t="s">
+        <v>13</v>
+      </c>
+      <c r="J178" t="s">
+        <v>13</v>
+      </c>
+      <c r="K178" t="s">
+        <v>32</v>
+      </c>
+      <c r="L178" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" ht="32">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179" t="s">
+        <v>10</v>
+      </c>
+      <c r="C179">
+        <v>2013</v>
+      </c>
+      <c r="E179">
+        <v>5</v>
+      </c>
+      <c r="G179" t="s">
+        <v>473</v>
+      </c>
+      <c r="H179" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="I179" t="s">
+        <v>19</v>
+      </c>
+      <c r="J179" t="s">
+        <v>32</v>
+      </c>
+      <c r="K179" t="s">
+        <v>32</v>
+      </c>
+      <c r="L179" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" ht="32">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180" t="s">
+        <v>10</v>
+      </c>
+      <c r="C180">
+        <v>2013</v>
+      </c>
+      <c r="E180">
+        <v>5</v>
+      </c>
+      <c r="G180" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="H180" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="I180" t="s">
+        <v>13</v>
+      </c>
+      <c r="J180" t="s">
+        <v>19</v>
+      </c>
+      <c r="K180" t="s">
+        <v>13</v>
+      </c>
+      <c r="L180" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" ht="32">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181" t="s">
+        <v>10</v>
+      </c>
+      <c r="C181">
+        <v>2013</v>
+      </c>
+      <c r="E181">
+        <v>5</v>
+      </c>
+      <c r="G181" t="s">
+        <v>477</v>
+      </c>
+      <c r="H181" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="I181" t="s">
+        <v>13</v>
+      </c>
+      <c r="J181" t="s">
+        <v>13</v>
+      </c>
+      <c r="K181" t="s">
+        <v>32</v>
+      </c>
+      <c r="L181" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" ht="32">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182" t="s">
+        <v>10</v>
+      </c>
+      <c r="C182">
+        <v>2013</v>
+      </c>
+      <c r="E182">
+        <v>5</v>
+      </c>
+      <c r="G182" t="s">
+        <v>479</v>
+      </c>
+      <c r="H182" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="I182" t="s">
+        <v>13</v>
+      </c>
+      <c r="J182" t="s">
+        <v>13</v>
+      </c>
+      <c r="K182" t="s">
+        <v>32</v>
+      </c>
+      <c r="L182" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" ht="32">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183" t="s">
+        <v>10</v>
+      </c>
+      <c r="C183">
+        <v>2013</v>
+      </c>
+      <c r="E183">
+        <v>5</v>
+      </c>
+      <c r="G183" t="s">
+        <v>481</v>
+      </c>
+      <c r="H183" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="I183" t="s">
+        <v>13</v>
+      </c>
+      <c r="J183" t="s">
+        <v>13</v>
+      </c>
+      <c r="K183" t="s">
+        <v>32</v>
+      </c>
+      <c r="L183" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" ht="32">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184" t="s">
+        <v>10</v>
+      </c>
+      <c r="C184">
+        <v>2013</v>
+      </c>
+      <c r="E184">
+        <v>5</v>
+      </c>
+      <c r="G184" t="s">
+        <v>483</v>
+      </c>
+      <c r="H184" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="I184" t="s">
+        <v>19</v>
+      </c>
+      <c r="J184" t="s">
+        <v>32</v>
+      </c>
+      <c r="K184" t="s">
+        <v>32</v>
+      </c>
+      <c r="L184" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" ht="32">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185" t="s">
+        <v>10</v>
+      </c>
+      <c r="C185">
+        <v>2013</v>
+      </c>
+      <c r="E185">
+        <v>5</v>
+      </c>
+      <c r="G185" t="s">
+        <v>485</v>
+      </c>
+      <c r="H185" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="I185" t="s">
+        <v>13</v>
+      </c>
+      <c r="J185" t="s">
+        <v>13</v>
+      </c>
+      <c r="K185" t="s">
+        <v>32</v>
+      </c>
+      <c r="L185" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" ht="32">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186" t="s">
+        <v>10</v>
+      </c>
+      <c r="C186">
+        <v>2013</v>
+      </c>
+      <c r="E186">
+        <v>4</v>
+      </c>
+      <c r="G186" t="s">
+        <v>487</v>
+      </c>
+      <c r="H186" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="I186" t="s">
+        <v>13</v>
+      </c>
+      <c r="J186" t="s">
+        <v>19</v>
+      </c>
+      <c r="K186" t="s">
+        <v>13</v>
+      </c>
+      <c r="L186" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" ht="32">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187" t="s">
+        <v>10</v>
+      </c>
+      <c r="C187">
+        <v>2013</v>
+      </c>
+      <c r="E187">
+        <v>4</v>
+      </c>
+      <c r="G187" t="s">
+        <v>489</v>
+      </c>
+      <c r="H187" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="I187" t="s">
+        <v>13</v>
+      </c>
+      <c r="J187" t="s">
+        <v>19</v>
+      </c>
+      <c r="K187" t="s">
+        <v>13</v>
+      </c>
+      <c r="L187" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" ht="32">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188" t="s">
+        <v>10</v>
+      </c>
+      <c r="C188">
+        <v>2013</v>
+      </c>
+      <c r="E188">
+        <v>4</v>
+      </c>
+      <c r="G188" t="s">
+        <v>491</v>
+      </c>
+      <c r="H188" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="I188" t="s">
+        <v>13</v>
+      </c>
+      <c r="J188" t="s">
+        <v>13</v>
+      </c>
+      <c r="K188" t="s">
+        <v>32</v>
+      </c>
+      <c r="L188" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" ht="32">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189" t="s">
+        <v>10</v>
+      </c>
+      <c r="C189">
+        <v>2013</v>
+      </c>
+      <c r="E189">
+        <v>4</v>
+      </c>
+      <c r="G189" t="s">
+        <v>493</v>
+      </c>
+      <c r="H189" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="I189" t="s">
+        <v>13</v>
+      </c>
+      <c r="J189" t="s">
+        <v>13</v>
+      </c>
+      <c r="K189" t="s">
+        <v>32</v>
+      </c>
+      <c r="L189" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" ht="32">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190" t="s">
+        <v>10</v>
+      </c>
+      <c r="C190">
+        <v>2013</v>
+      </c>
+      <c r="E190">
+        <v>4</v>
+      </c>
+      <c r="G190" t="s">
+        <v>495</v>
+      </c>
+      <c r="H190" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="I190" t="s">
+        <v>19</v>
+      </c>
+      <c r="J190" t="s">
+        <v>13</v>
+      </c>
+      <c r="K190" t="s">
+        <v>32</v>
+      </c>
+      <c r="L190" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" ht="32">
+      <c r="A191">
+        <v>190</v>
+      </c>
+      <c r="B191" t="s">
+        <v>10</v>
+      </c>
+      <c r="C191">
+        <v>2013</v>
+      </c>
+      <c r="E191">
+        <v>4</v>
+      </c>
+      <c r="G191" t="s">
+        <v>497</v>
+      </c>
+      <c r="H191" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="I191" t="s">
+        <v>19</v>
+      </c>
+      <c r="J191" t="s">
+        <v>13</v>
+      </c>
+      <c r="K191" t="s">
+        <v>32</v>
+      </c>
+      <c r="L191" t="s">
+        <v>33</v>
+      </c>
+      <c r="M191" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" ht="32">
+      <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192" t="s">
+        <v>10</v>
+      </c>
+      <c r="C192">
+        <v>2013</v>
+      </c>
+      <c r="E192">
+        <v>4</v>
+      </c>
+      <c r="G192" t="s">
+        <v>500</v>
+      </c>
+      <c r="H192" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="I192" t="s">
+        <v>13</v>
+      </c>
+      <c r="J192" t="s">
+        <v>19</v>
+      </c>
+      <c r="K192" t="s">
+        <v>13</v>
+      </c>
+      <c r="L192" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" ht="32">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193" t="s">
+        <v>10</v>
+      </c>
+      <c r="C193">
+        <v>2013</v>
+      </c>
+      <c r="E193">
+        <v>4</v>
+      </c>
+      <c r="G193" t="s">
+        <v>502</v>
+      </c>
+      <c r="H193" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="I193" t="s">
+        <v>13</v>
+      </c>
+      <c r="J193" t="s">
+        <v>19</v>
+      </c>
+      <c r="K193" t="s">
+        <v>13</v>
+      </c>
+      <c r="L193" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" ht="32">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194" t="s">
+        <v>10</v>
+      </c>
+      <c r="C194">
+        <v>2013</v>
+      </c>
+      <c r="E194">
+        <v>4</v>
+      </c>
+      <c r="G194" t="s">
+        <v>504</v>
+      </c>
+      <c r="H194" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="I194" t="s">
+        <v>13</v>
+      </c>
+      <c r="J194" t="s">
+        <v>19</v>
+      </c>
+      <c r="K194" t="s">
+        <v>13</v>
+      </c>
+      <c r="L194" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" ht="32">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195" t="s">
+        <v>10</v>
+      </c>
+      <c r="C195">
+        <v>2013</v>
+      </c>
+      <c r="E195">
+        <v>4</v>
+      </c>
+      <c r="G195" t="s">
+        <v>506</v>
+      </c>
+      <c r="H195" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="I195" t="s">
+        <v>13</v>
+      </c>
+      <c r="J195" t="s">
+        <v>13</v>
+      </c>
+      <c r="K195" t="s">
+        <v>32</v>
+      </c>
+      <c r="L195" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" ht="32">
+      <c r="A196">
+        <v>195</v>
+      </c>
+      <c r="B196" t="s">
+        <v>10</v>
+      </c>
+      <c r="C196">
+        <v>2013</v>
+      </c>
+      <c r="E196">
+        <v>4</v>
+      </c>
+      <c r="G196" t="s">
+        <v>508</v>
+      </c>
+      <c r="H196" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="I196" t="s">
+        <v>19</v>
+      </c>
+      <c r="J196" t="s">
+        <v>32</v>
+      </c>
+      <c r="K196" t="s">
+        <v>32</v>
+      </c>
+      <c r="L196" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" ht="32">
+      <c r="A197">
+        <v>196</v>
+      </c>
+      <c r="B197" t="s">
+        <v>10</v>
+      </c>
+      <c r="C197">
+        <v>2013</v>
+      </c>
+      <c r="E197">
+        <v>4</v>
+      </c>
+      <c r="G197" t="s">
+        <v>510</v>
+      </c>
+      <c r="H197" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="I197" t="s">
+        <v>13</v>
+      </c>
+      <c r="J197" t="s">
+        <v>13</v>
+      </c>
+      <c r="K197" t="s">
+        <v>32</v>
+      </c>
+      <c r="L197" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" ht="32">
+      <c r="A198">
+        <v>197</v>
+      </c>
+      <c r="B198" t="s">
+        <v>10</v>
+      </c>
+      <c r="C198">
+        <v>2013</v>
+      </c>
+      <c r="E198">
+        <v>4</v>
+      </c>
+      <c r="G198" t="s">
+        <v>512</v>
+      </c>
+      <c r="H198" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="I198" t="s">
+        <v>19</v>
+      </c>
+      <c r="J198" t="s">
+        <v>32</v>
+      </c>
+      <c r="K198" t="s">
+        <v>32</v>
+      </c>
+      <c r="L198" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" ht="32">
+      <c r="A199">
+        <v>198</v>
+      </c>
+      <c r="B199" t="s">
+        <v>10</v>
+      </c>
+      <c r="C199">
+        <v>2013</v>
+      </c>
+      <c r="E199">
+        <v>4</v>
+      </c>
+      <c r="G199" t="s">
+        <v>514</v>
+      </c>
+      <c r="H199" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="I199" t="s">
+        <v>19</v>
+      </c>
+      <c r="J199" t="s">
+        <v>32</v>
+      </c>
+      <c r="K199" t="s">
+        <v>32</v>
+      </c>
+      <c r="L199" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" ht="32">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200" t="s">
+        <v>10</v>
+      </c>
+      <c r="C200">
+        <v>2013</v>
+      </c>
+      <c r="E200">
+        <v>3</v>
+      </c>
+      <c r="G200" t="s">
+        <v>516</v>
+      </c>
+      <c r="H200" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="I200" t="s">
+        <v>13</v>
+      </c>
+      <c r="J200" t="s">
+        <v>13</v>
+      </c>
+      <c r="K200" t="s">
+        <v>32</v>
+      </c>
+      <c r="L200" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" ht="32">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201" t="s">
+        <v>10</v>
+      </c>
+      <c r="C201">
+        <v>2013</v>
+      </c>
+      <c r="E201">
+        <v>3</v>
+      </c>
+      <c r="G201" t="s">
+        <v>518</v>
+      </c>
+      <c r="H201" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="I201" t="s">
+        <v>13</v>
+      </c>
+      <c r="J201" t="s">
+        <v>13</v>
+      </c>
+      <c r="K201" t="s">
+        <v>32</v>
+      </c>
+      <c r="L201" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" ht="32">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202" t="s">
+        <v>10</v>
+      </c>
+      <c r="C202">
+        <v>2013</v>
+      </c>
+      <c r="E202">
+        <v>3</v>
+      </c>
+      <c r="G202" t="s">
+        <v>520</v>
+      </c>
+      <c r="H202" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="I202" t="s">
+        <v>13</v>
+      </c>
+      <c r="J202" t="s">
+        <v>13</v>
+      </c>
+      <c r="K202" t="s">
+        <v>32</v>
+      </c>
+      <c r="L202" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" ht="32">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203" t="s">
+        <v>10</v>
+      </c>
+      <c r="C203">
+        <v>2013</v>
+      </c>
+      <c r="E203">
+        <v>3</v>
+      </c>
+      <c r="G203" t="s">
+        <v>522</v>
+      </c>
+      <c r="H203" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I203" t="s">
+        <v>13</v>
+      </c>
+      <c r="J203" t="s">
+        <v>13</v>
+      </c>
+      <c r="K203" t="s">
+        <v>32</v>
+      </c>
+      <c r="L203" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" ht="32">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204" t="s">
+        <v>10</v>
+      </c>
+      <c r="C204">
+        <v>2013</v>
+      </c>
+      <c r="E204">
+        <v>3</v>
+      </c>
+      <c r="G204" t="s">
+        <v>524</v>
+      </c>
+      <c r="H204" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="I204" t="s">
+        <v>13</v>
+      </c>
+      <c r="J204" t="s">
+        <v>19</v>
+      </c>
+      <c r="K204" t="s">
+        <v>13</v>
+      </c>
+      <c r="L204" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" ht="32">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205" t="s">
+        <v>10</v>
+      </c>
+      <c r="C205">
+        <v>2013</v>
+      </c>
+      <c r="E205">
+        <v>3</v>
+      </c>
+      <c r="G205" t="s">
+        <v>526</v>
+      </c>
+      <c r="H205" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="I205" t="s">
+        <v>13</v>
+      </c>
+      <c r="J205" t="s">
+        <v>19</v>
+      </c>
+      <c r="K205" t="s">
+        <v>13</v>
+      </c>
+      <c r="L205" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" ht="32">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206" t="s">
+        <v>10</v>
+      </c>
+      <c r="C206">
+        <v>2013</v>
+      </c>
+      <c r="E206">
+        <v>3</v>
+      </c>
+      <c r="G206" t="s">
+        <v>528</v>
+      </c>
+      <c r="H206" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="I206" t="s">
+        <v>13</v>
+      </c>
+      <c r="J206" t="s">
+        <v>13</v>
+      </c>
+      <c r="K206" t="s">
+        <v>32</v>
+      </c>
+      <c r="L206" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" ht="32">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207" t="s">
+        <v>10</v>
+      </c>
+      <c r="C207">
+        <v>2013</v>
+      </c>
+      <c r="E207">
+        <v>3</v>
+      </c>
+      <c r="G207" t="s">
+        <v>530</v>
+      </c>
+      <c r="H207" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="I207" t="s">
+        <v>13</v>
+      </c>
+      <c r="J207" t="s">
+        <v>13</v>
+      </c>
+      <c r="K207" t="s">
+        <v>32</v>
+      </c>
+      <c r="L207" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" ht="32">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208" t="s">
+        <v>10</v>
+      </c>
+      <c r="C208">
+        <v>2013</v>
+      </c>
+      <c r="E208">
+        <v>3</v>
+      </c>
+      <c r="G208" t="s">
+        <v>532</v>
+      </c>
+      <c r="H208" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="I208" t="s">
+        <v>13</v>
+      </c>
+      <c r="J208" t="s">
+        <v>13</v>
+      </c>
+      <c r="K208" t="s">
+        <v>32</v>
+      </c>
+      <c r="L208" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" ht="32">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209" t="s">
+        <v>10</v>
+      </c>
+      <c r="C209">
+        <v>2013</v>
+      </c>
+      <c r="E209">
+        <v>3</v>
+      </c>
+      <c r="G209" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="H209" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="I209" t="s">
+        <v>13</v>
+      </c>
+      <c r="J209" t="s">
+        <v>13</v>
+      </c>
+      <c r="K209" t="s">
+        <v>32</v>
+      </c>
+      <c r="L209" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" ht="32">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210" t="s">
+        <v>10</v>
+      </c>
+      <c r="C210">
+        <v>2013</v>
+      </c>
+      <c r="E210">
+        <v>3</v>
+      </c>
+      <c r="G210" t="s">
+        <v>536</v>
+      </c>
+      <c r="H210" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="I210" t="s">
+        <v>19</v>
+      </c>
+      <c r="J210" t="s">
+        <v>32</v>
+      </c>
+      <c r="K210" t="s">
+        <v>32</v>
+      </c>
+      <c r="L210" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" ht="32">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211" t="s">
+        <v>10</v>
+      </c>
+      <c r="C211">
+        <v>2013</v>
+      </c>
+      <c r="E211">
+        <v>3</v>
+      </c>
+      <c r="G211" t="s">
+        <v>538</v>
+      </c>
+      <c r="H211" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="I211" t="s">
+        <v>13</v>
+      </c>
+      <c r="J211" t="s">
+        <v>13</v>
+      </c>
+      <c r="K211" t="s">
+        <v>32</v>
+      </c>
+      <c r="L211" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" ht="32">
+      <c r="A212">
+        <v>211</v>
+      </c>
+      <c r="B212" t="s">
+        <v>10</v>
+      </c>
+      <c r="C212">
+        <v>2013</v>
+      </c>
+      <c r="E212">
+        <v>3</v>
+      </c>
+      <c r="G212" t="s">
+        <v>540</v>
+      </c>
+      <c r="H212" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="I212" t="s">
+        <v>13</v>
+      </c>
+      <c r="J212" t="s">
+        <v>19</v>
+      </c>
+      <c r="K212" t="s">
+        <v>13</v>
+      </c>
+      <c r="L212" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" ht="32">
+      <c r="A213">
+        <v>212</v>
+      </c>
+      <c r="B213" t="s">
+        <v>10</v>
+      </c>
+      <c r="C213">
+        <v>2013</v>
+      </c>
+      <c r="E213">
+        <v>3</v>
+      </c>
+      <c r="G213" t="s">
+        <v>542</v>
+      </c>
+      <c r="H213" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="I213" t="s">
+        <v>19</v>
+      </c>
+      <c r="J213" t="s">
+        <v>32</v>
+      </c>
+      <c r="K213" t="s">
+        <v>32</v>
+      </c>
+      <c r="L213" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" ht="32">
+      <c r="A214">
+        <v>213</v>
+      </c>
+      <c r="B214" t="s">
+        <v>10</v>
+      </c>
+      <c r="C214">
+        <v>2013</v>
+      </c>
+      <c r="E214">
+        <v>3</v>
+      </c>
+      <c r="G214" t="s">
+        <v>544</v>
+      </c>
+      <c r="H214" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="I214" t="s">
+        <v>13</v>
+      </c>
+      <c r="J214" t="s">
+        <v>19</v>
+      </c>
+      <c r="K214" t="s">
+        <v>13</v>
+      </c>
+      <c r="L214" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" ht="32">
+      <c r="A215">
+        <v>214</v>
+      </c>
+      <c r="B215" t="s">
+        <v>10</v>
+      </c>
+      <c r="C215">
+        <v>2013</v>
+      </c>
+      <c r="E215">
+        <v>3</v>
+      </c>
+      <c r="G215" t="s">
+        <v>546</v>
+      </c>
+      <c r="H215" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="I215" t="s">
+        <v>19</v>
+      </c>
+      <c r="J215" t="s">
+        <v>32</v>
+      </c>
+      <c r="K215" t="s">
+        <v>32</v>
+      </c>
+      <c r="L215" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" ht="32">
+      <c r="A216">
+        <v>215</v>
+      </c>
+      <c r="B216" t="s">
+        <v>10</v>
+      </c>
+      <c r="C216">
+        <v>2013</v>
+      </c>
+      <c r="E216">
+        <v>3</v>
+      </c>
+      <c r="G216" t="s">
+        <v>548</v>
+      </c>
+      <c r="H216" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="I216" t="s">
+        <v>19</v>
+      </c>
+      <c r="J216" t="s">
+        <v>32</v>
+      </c>
+      <c r="K216" t="s">
+        <v>32</v>
+      </c>
+      <c r="L216" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" ht="32">
+      <c r="A217">
+        <v>216</v>
+      </c>
+      <c r="B217" t="s">
+        <v>10</v>
+      </c>
+      <c r="C217">
+        <v>2013</v>
+      </c>
+      <c r="E217">
+        <v>3</v>
+      </c>
+      <c r="G217" t="s">
+        <v>550</v>
+      </c>
+      <c r="H217" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="I217" t="s">
+        <v>13</v>
+      </c>
+      <c r="J217" t="s">
+        <v>13</v>
+      </c>
+      <c r="K217" t="s">
+        <v>32</v>
+      </c>
+      <c r="L217" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" ht="32">
+      <c r="A218">
+        <v>217</v>
+      </c>
+      <c r="B218" t="s">
+        <v>10</v>
+      </c>
+      <c r="C218">
+        <v>2013</v>
+      </c>
+      <c r="E218">
+        <v>3</v>
+      </c>
+      <c r="G218" t="s">
+        <v>552</v>
+      </c>
+      <c r="H218" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="I218" t="s">
+        <v>13</v>
+      </c>
+      <c r="J218" t="s">
+        <v>13</v>
+      </c>
+      <c r="K218" t="s">
+        <v>32</v>
+      </c>
+      <c r="L218" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" ht="32">
+      <c r="A219">
+        <v>218</v>
+      </c>
+      <c r="B219" t="s">
+        <v>10</v>
+      </c>
+      <c r="C219">
+        <v>2013</v>
+      </c>
+      <c r="E219">
+        <v>3</v>
+      </c>
+      <c r="G219" t="s">
+        <v>554</v>
+      </c>
+      <c r="H219" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="I219" t="s">
+        <v>19</v>
+      </c>
+      <c r="J219" t="s">
+        <v>13</v>
+      </c>
+      <c r="K219" t="s">
+        <v>32</v>
+      </c>
+      <c r="L219" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" ht="32">
+      <c r="A220">
+        <v>219</v>
+      </c>
+      <c r="B220" t="s">
+        <v>10</v>
+      </c>
+      <c r="C220">
+        <v>2013</v>
+      </c>
+      <c r="E220">
+        <v>3</v>
+      </c>
+      <c r="G220" t="s">
+        <v>556</v>
+      </c>
+      <c r="H220" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="I220" t="s">
+        <v>19</v>
+      </c>
+      <c r="J220" t="s">
+        <v>32</v>
+      </c>
+      <c r="K220" t="s">
+        <v>32</v>
+      </c>
+      <c r="L220" t="s">
+        <v>32</v>
+      </c>
+      <c r="M220" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" ht="32">
+      <c r="A221">
+        <v>220</v>
+      </c>
+      <c r="B221" t="s">
+        <v>10</v>
+      </c>
+      <c r="C221">
+        <v>2013</v>
+      </c>
+      <c r="E221">
+        <v>3</v>
+      </c>
+      <c r="G221" t="s">
+        <v>559</v>
+      </c>
+      <c r="H221" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="I221" t="s">
+        <v>19</v>
+      </c>
+      <c r="J221" t="s">
+        <v>32</v>
+      </c>
+      <c r="K221" t="s">
+        <v>32</v>
+      </c>
+      <c r="L221" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" ht="32">
+      <c r="A222">
+        <v>221</v>
+      </c>
+      <c r="B222" t="s">
+        <v>10</v>
+      </c>
+      <c r="C222">
+        <v>2013</v>
+      </c>
+      <c r="E222">
+        <v>3</v>
+      </c>
+      <c r="G222" t="s">
+        <v>561</v>
+      </c>
+      <c r="H222" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="I222" t="s">
+        <v>13</v>
+      </c>
+      <c r="J222" t="s">
+        <v>13</v>
+      </c>
+      <c r="K222" t="s">
+        <v>32</v>
+      </c>
+      <c r="L222" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" ht="32">
+      <c r="A223">
+        <v>222</v>
+      </c>
+      <c r="B223" t="s">
+        <v>10</v>
+      </c>
+      <c r="C223">
+        <v>2013</v>
+      </c>
+      <c r="E223">
+        <v>2</v>
+      </c>
+      <c r="G223" t="s">
+        <v>563</v>
+      </c>
+      <c r="H223" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="I223" t="s">
+        <v>13</v>
+      </c>
+      <c r="J223" t="s">
+        <v>13</v>
+      </c>
+      <c r="K223" t="s">
+        <v>32</v>
+      </c>
+      <c r="L223" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" ht="32">
+      <c r="A224">
+        <v>223</v>
+      </c>
+      <c r="B224" t="s">
+        <v>10</v>
+      </c>
+      <c r="C224">
+        <v>2013</v>
+      </c>
+      <c r="E224">
+        <v>2</v>
+      </c>
+      <c r="G224" t="s">
+        <v>565</v>
+      </c>
+      <c r="H224" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="I224" t="s">
+        <v>13</v>
+      </c>
+      <c r="J224" t="s">
+        <v>13</v>
+      </c>
+      <c r="K224" t="s">
+        <v>32</v>
+      </c>
+      <c r="L224" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" ht="32">
+      <c r="A225">
+        <v>224</v>
+      </c>
+      <c r="B225" t="s">
+        <v>10</v>
+      </c>
+      <c r="C225">
+        <v>2013</v>
+      </c>
+      <c r="E225">
+        <v>2</v>
+      </c>
+      <c r="G225" t="s">
+        <v>567</v>
+      </c>
+      <c r="H225" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="I225" t="s">
+        <v>13</v>
+      </c>
+      <c r="J225" t="s">
+        <v>13</v>
+      </c>
+      <c r="K225" t="s">
+        <v>32</v>
+      </c>
+      <c r="L225" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" ht="32">
+      <c r="A226">
+        <v>225</v>
+      </c>
+      <c r="B226" t="s">
+        <v>10</v>
+      </c>
+      <c r="C226">
+        <v>2013</v>
+      </c>
+      <c r="E226">
+        <v>2</v>
+      </c>
+      <c r="G226" t="s">
+        <v>569</v>
+      </c>
+      <c r="H226" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="I226" t="s">
+        <v>13</v>
+      </c>
+      <c r="J226" t="s">
+        <v>13</v>
+      </c>
+      <c r="K226" t="s">
+        <v>32</v>
+      </c>
+      <c r="L226" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" ht="32">
+      <c r="A227">
+        <v>226</v>
+      </c>
+      <c r="B227" t="s">
+        <v>10</v>
+      </c>
+      <c r="C227">
+        <v>2013</v>
+      </c>
+      <c r="E227">
+        <v>2</v>
+      </c>
+      <c r="G227" t="s">
+        <v>571</v>
+      </c>
+      <c r="H227" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="I227" t="s">
+        <v>13</v>
+      </c>
+      <c r="J227" t="s">
+        <v>13</v>
+      </c>
+      <c r="K227" t="s">
+        <v>32</v>
+      </c>
+      <c r="L227" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" ht="32">
+      <c r="A228">
+        <v>227</v>
+      </c>
+      <c r="B228" t="s">
+        <v>10</v>
+      </c>
+      <c r="C228">
+        <v>2013</v>
+      </c>
+      <c r="E228">
+        <v>2</v>
+      </c>
+      <c r="G228" t="s">
+        <v>573</v>
+      </c>
+      <c r="H228" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="I228" t="s">
+        <v>19</v>
+      </c>
+      <c r="J228" t="s">
+        <v>32</v>
+      </c>
+      <c r="K228" t="s">
+        <v>32</v>
+      </c>
+      <c r="L228" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" ht="32">
+      <c r="A229">
+        <v>228</v>
+      </c>
+      <c r="B229" t="s">
+        <v>10</v>
+      </c>
+      <c r="C229">
+        <v>2013</v>
+      </c>
+      <c r="E229">
+        <v>2</v>
+      </c>
+      <c r="G229" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="H229" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="I229" t="s">
+        <v>13</v>
+      </c>
+      <c r="J229" t="s">
+        <v>13</v>
+      </c>
+      <c r="K229" t="s">
+        <v>32</v>
+      </c>
+      <c r="L229" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" ht="32">
+      <c r="A230">
+        <v>229</v>
+      </c>
+      <c r="B230" t="s">
+        <v>10</v>
+      </c>
+      <c r="C230">
+        <v>2013</v>
+      </c>
+      <c r="E230">
+        <v>2</v>
+      </c>
+      <c r="G230" t="s">
+        <v>577</v>
+      </c>
+      <c r="H230" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="I230" t="s">
+        <v>13</v>
+      </c>
+      <c r="J230" t="s">
+        <v>13</v>
+      </c>
+      <c r="K230" t="s">
+        <v>32</v>
+      </c>
+      <c r="L230" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" ht="32">
+      <c r="A231">
+        <v>230</v>
+      </c>
+      <c r="B231" t="s">
+        <v>10</v>
+      </c>
+      <c r="C231">
+        <v>2013</v>
+      </c>
+      <c r="E231">
+        <v>2</v>
+      </c>
+      <c r="G231" t="s">
+        <v>532</v>
+      </c>
+      <c r="H231" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="I231" t="s">
+        <v>19</v>
+      </c>
+      <c r="J231" t="s">
+        <v>32</v>
+      </c>
+      <c r="K231" t="s">
+        <v>32</v>
+      </c>
+      <c r="L231" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" ht="32">
+      <c r="A232">
+        <v>231</v>
+      </c>
+      <c r="B232" t="s">
+        <v>10</v>
+      </c>
+      <c r="C232">
+        <v>2013</v>
+      </c>
+      <c r="E232">
+        <v>2</v>
+      </c>
+      <c r="G232" t="s">
+        <v>580</v>
+      </c>
+      <c r="H232" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="I232" t="s">
+        <v>13</v>
+      </c>
+      <c r="J232" t="s">
+        <v>13</v>
+      </c>
+      <c r="K232" t="s">
+        <v>32</v>
+      </c>
+      <c r="L232" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" ht="32">
+      <c r="A233">
+        <v>232</v>
+      </c>
+      <c r="B233" t="s">
+        <v>10</v>
+      </c>
+      <c r="C233">
+        <v>2013</v>
+      </c>
+      <c r="E233">
+        <v>2</v>
+      </c>
+      <c r="G233" t="s">
+        <v>582</v>
+      </c>
+      <c r="H233" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="I233" t="s">
+        <v>19</v>
+      </c>
+      <c r="J233" t="s">
+        <v>32</v>
+      </c>
+      <c r="K233" t="s">
+        <v>32</v>
+      </c>
+      <c r="L233" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" ht="32">
+      <c r="A234">
+        <v>233</v>
+      </c>
+      <c r="B234" t="s">
+        <v>10</v>
+      </c>
+      <c r="C234">
+        <v>2013</v>
+      </c>
+      <c r="E234">
+        <v>2</v>
+      </c>
+      <c r="G234" t="s">
+        <v>584</v>
+      </c>
+      <c r="H234" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="I234" t="s">
+        <v>13</v>
+      </c>
+      <c r="J234" t="s">
+        <v>13</v>
+      </c>
+      <c r="K234" t="s">
+        <v>32</v>
+      </c>
+      <c r="L234" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" ht="32">
+      <c r="A235">
+        <v>234</v>
+      </c>
+      <c r="B235" t="s">
+        <v>10</v>
+      </c>
+      <c r="C235">
+        <v>2013</v>
+      </c>
+      <c r="E235">
+        <v>2</v>
+      </c>
+      <c r="G235" t="s">
+        <v>586</v>
+      </c>
+      <c r="H235" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="I235" t="s">
+        <v>13</v>
+      </c>
+      <c r="J235" t="s">
+        <v>19</v>
+      </c>
+      <c r="K235" t="s">
+        <v>19</v>
+      </c>
+      <c r="L235" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" ht="32">
+      <c r="A236">
+        <v>235</v>
+      </c>
+      <c r="B236" t="s">
+        <v>10</v>
+      </c>
+      <c r="C236">
+        <v>2013</v>
+      </c>
+      <c r="E236">
+        <v>2</v>
+      </c>
+      <c r="G236" t="s">
+        <v>588</v>
+      </c>
+      <c r="H236" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="I236" t="s">
+        <v>19</v>
+      </c>
+      <c r="J236" t="s">
+        <v>13</v>
+      </c>
+      <c r="K236" t="s">
+        <v>32</v>
+      </c>
+      <c r="L236" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" ht="32">
+      <c r="A237">
+        <v>236</v>
+      </c>
+      <c r="B237" t="s">
+        <v>10</v>
+      </c>
+      <c r="C237">
+        <v>2013</v>
+      </c>
+      <c r="E237">
+        <v>2</v>
+      </c>
+      <c r="G237" t="s">
+        <v>590</v>
+      </c>
+      <c r="H237" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="I237" t="s">
+        <v>13</v>
+      </c>
+      <c r="J237" t="s">
+        <v>13</v>
+      </c>
+      <c r="K237" t="s">
+        <v>32</v>
+      </c>
+      <c r="L237" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" ht="32">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238" t="s">
+        <v>10</v>
+      </c>
+      <c r="C238">
+        <v>2013</v>
+      </c>
+      <c r="E238">
+        <v>2</v>
+      </c>
+      <c r="G238" t="s">
+        <v>592</v>
+      </c>
+      <c r="H238" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="I238" t="s">
+        <v>13</v>
+      </c>
+      <c r="J238" t="s">
+        <v>13</v>
+      </c>
+      <c r="K238" t="s">
+        <v>32</v>
+      </c>
+      <c r="L238" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" ht="32">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239" t="s">
+        <v>10</v>
+      </c>
+      <c r="C239">
+        <v>2013</v>
+      </c>
+      <c r="E239">
+        <v>2</v>
+      </c>
+      <c r="G239" t="s">
+        <v>594</v>
+      </c>
+      <c r="H239" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="I239" t="s">
+        <v>19</v>
+      </c>
+      <c r="J239" t="s">
+        <v>32</v>
+      </c>
+      <c r="K239" t="s">
+        <v>32</v>
+      </c>
+      <c r="L239" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" ht="32">
+      <c r="A240">
+        <v>239</v>
+      </c>
+      <c r="B240" t="s">
+        <v>10</v>
+      </c>
+      <c r="C240">
+        <v>2013</v>
+      </c>
+      <c r="E240">
+        <v>2</v>
+      </c>
+      <c r="G240" t="s">
+        <v>596</v>
+      </c>
+      <c r="H240" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="I240" t="s">
+        <v>13</v>
+      </c>
+      <c r="J240" t="s">
+        <v>13</v>
+      </c>
+      <c r="K240" t="s">
+        <v>32</v>
+      </c>
+      <c r="L240" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12" ht="32">
+      <c r="A241">
+        <v>240</v>
+      </c>
+      <c r="B241" t="s">
+        <v>10</v>
+      </c>
+      <c r="C241">
+        <v>2013</v>
+      </c>
+      <c r="E241">
+        <v>1</v>
+      </c>
+      <c r="G241" t="s">
+        <v>598</v>
+      </c>
+      <c r="H241" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="I241" t="s">
+        <v>19</v>
+      </c>
+      <c r="J241" t="s">
+        <v>32</v>
+      </c>
+      <c r="K241" t="s">
+        <v>32</v>
+      </c>
+      <c r="L241" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" ht="32">
+      <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242" t="s">
+        <v>10</v>
+      </c>
+      <c r="C242">
+        <v>2013</v>
+      </c>
+      <c r="E242">
+        <v>1</v>
+      </c>
+      <c r="G242" t="s">
+        <v>601</v>
+      </c>
+      <c r="H242" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="I242" t="s">
+        <v>13</v>
+      </c>
+      <c r="J242" t="s">
+        <v>13</v>
+      </c>
+      <c r="K242" t="s">
+        <v>32</v>
+      </c>
+      <c r="L242" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" ht="32">
+      <c r="A243">
+        <v>242</v>
+      </c>
+      <c r="B243" t="s">
+        <v>10</v>
+      </c>
+      <c r="C243">
+        <v>2013</v>
+      </c>
+      <c r="E243">
+        <v>1</v>
+      </c>
+      <c r="G243" t="s">
+        <v>602</v>
+      </c>
+      <c r="H243" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="I243" t="s">
+        <v>13</v>
+      </c>
+      <c r="J243" t="s">
+        <v>13</v>
+      </c>
+      <c r="K243" t="s">
+        <v>32</v>
+      </c>
+      <c r="L243" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" ht="32">
+      <c r="A244">
+        <v>243</v>
+      </c>
+      <c r="B244" t="s">
+        <v>10</v>
+      </c>
+      <c r="C244">
+        <v>2013</v>
+      </c>
+      <c r="E244">
+        <v>1</v>
+      </c>
+      <c r="G244" t="s">
+        <v>604</v>
+      </c>
+      <c r="H244" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="I244" t="s">
+        <v>19</v>
+      </c>
+      <c r="J244" t="s">
+        <v>32</v>
+      </c>
+      <c r="K244" t="s">
+        <v>32</v>
+      </c>
+      <c r="L244" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" ht="32">
+      <c r="A245">
+        <v>244</v>
+      </c>
+      <c r="B245" t="s">
+        <v>10</v>
+      </c>
+      <c r="C245">
+        <v>2013</v>
+      </c>
+      <c r="E245">
+        <v>1</v>
+      </c>
+      <c r="G245" t="s">
+        <v>606</v>
+      </c>
+      <c r="H245" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="I245" t="s">
+        <v>13</v>
+      </c>
+      <c r="J245" t="s">
+        <v>13</v>
+      </c>
+      <c r="K245" t="s">
+        <v>32</v>
+      </c>
+      <c r="L245" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12" ht="32">
+      <c r="A246">
+        <v>245</v>
+      </c>
+      <c r="B246" t="s">
+        <v>10</v>
+      </c>
+      <c r="C246">
+        <v>2013</v>
+      </c>
+      <c r="E246">
+        <v>1</v>
+      </c>
+      <c r="G246" t="s">
+        <v>608</v>
+      </c>
+      <c r="H246" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="I246" t="s">
+        <v>13</v>
+      </c>
+      <c r="J246" t="s">
+        <v>19</v>
+      </c>
+      <c r="K246" t="s">
+        <v>13</v>
+      </c>
+      <c r="L246" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" ht="32">
+      <c r="A247">
+        <v>246</v>
+      </c>
+      <c r="B247" t="s">
+        <v>10</v>
+      </c>
+      <c r="C247">
+        <v>2013</v>
+      </c>
+      <c r="E247">
+        <v>1</v>
+      </c>
+      <c r="G247" t="s">
+        <v>610</v>
+      </c>
+      <c r="H247" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="I247" t="s">
+        <v>13</v>
+      </c>
+      <c r="J247" t="s">
+        <v>13</v>
+      </c>
+      <c r="K247" t="s">
+        <v>32</v>
+      </c>
+      <c r="L247" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" ht="32">
+      <c r="A248">
+        <v>247</v>
+      </c>
+      <c r="B248" t="s">
+        <v>10</v>
+      </c>
+      <c r="C248">
+        <v>2013</v>
+      </c>
+      <c r="E248">
+        <v>1</v>
+      </c>
+      <c r="G248" t="s">
+        <v>613</v>
+      </c>
+      <c r="H248" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="I248" t="s">
+        <v>13</v>
+      </c>
+      <c r="J248" t="s">
+        <v>13</v>
+      </c>
+      <c r="K248" t="s">
+        <v>32</v>
+      </c>
+      <c r="L248" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" ht="32">
+      <c r="A249">
+        <v>248</v>
+      </c>
+      <c r="B249" t="s">
+        <v>10</v>
+      </c>
+      <c r="C249">
+        <v>2013</v>
+      </c>
+      <c r="E249">
+        <v>1</v>
+      </c>
+      <c r="G249" t="s">
+        <v>614</v>
+      </c>
+      <c r="H249" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="I249" t="s">
+        <v>13</v>
+      </c>
+      <c r="J249" t="s">
+        <v>13</v>
+      </c>
+      <c r="K249" t="s">
+        <v>32</v>
+      </c>
+      <c r="L249" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" ht="32">
+      <c r="A250">
+        <v>249</v>
+      </c>
+      <c r="B250" t="s">
+        <v>10</v>
+      </c>
+      <c r="C250">
+        <v>2013</v>
+      </c>
+      <c r="E250">
+        <v>1</v>
+      </c>
+      <c r="G250" t="s">
+        <v>616</v>
+      </c>
+      <c r="H250" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="I250" t="s">
+        <v>13</v>
+      </c>
+      <c r="J250" t="s">
+        <v>19</v>
+      </c>
+      <c r="K250" t="s">
+        <v>13</v>
+      </c>
+      <c r="L250" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" ht="32">
+      <c r="A251">
+        <v>250</v>
+      </c>
+      <c r="B251" t="s">
+        <v>10</v>
+      </c>
+      <c r="C251">
+        <v>2013</v>
+      </c>
+      <c r="E251">
+        <v>1</v>
+      </c>
+      <c r="G251" t="s">
+        <v>408</v>
+      </c>
+      <c r="H251" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="I251" t="s">
+        <v>19</v>
+      </c>
+      <c r="J251" t="s">
+        <v>13</v>
+      </c>
+      <c r="K251" t="s">
+        <v>32</v>
+      </c>
+      <c r="L251" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" ht="32">
+      <c r="A252">
+        <v>251</v>
+      </c>
+      <c r="B252" t="s">
+        <v>10</v>
+      </c>
+      <c r="C252">
+        <v>2013</v>
+      </c>
+      <c r="E252">
+        <v>1</v>
+      </c>
+      <c r="G252" t="s">
+        <v>619</v>
+      </c>
+      <c r="H252" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="I252" t="s">
+        <v>621</v>
+      </c>
+      <c r="J252" t="s">
+        <v>13</v>
+      </c>
+      <c r="K252" t="s">
+        <v>32</v>
+      </c>
+      <c r="L252" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" ht="32">
+      <c r="A253">
+        <v>252</v>
+      </c>
+      <c r="B253" t="s">
+        <v>10</v>
+      </c>
+      <c r="C253">
+        <v>2013</v>
+      </c>
+      <c r="E253">
+        <v>1</v>
+      </c>
+      <c r="G253" t="s">
+        <v>622</v>
+      </c>
+      <c r="H253" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="I253" t="s">
+        <v>19</v>
+      </c>
+      <c r="J253" t="s">
+        <v>32</v>
+      </c>
+      <c r="K253" t="s">
+        <v>32</v>
+      </c>
+      <c r="L253" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" ht="32">
+      <c r="A254">
+        <v>253</v>
+      </c>
+      <c r="B254" t="s">
+        <v>10</v>
+      </c>
+      <c r="C254">
+        <v>2013</v>
+      </c>
+      <c r="E254">
+        <v>1</v>
+      </c>
+      <c r="G254" t="s">
+        <v>624</v>
+      </c>
+      <c r="H254" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="I254" t="s">
+        <v>13</v>
+      </c>
+      <c r="J254" t="s">
+        <v>13</v>
+      </c>
+      <c r="K254" t="s">
+        <v>32</v>
+      </c>
+      <c r="L254" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" ht="32">
+      <c r="A255">
+        <v>254</v>
+      </c>
+      <c r="B255" t="s">
+        <v>10</v>
+      </c>
+      <c r="C255">
+        <v>2013</v>
+      </c>
+      <c r="E255">
+        <v>1</v>
+      </c>
+      <c r="G255" t="s">
+        <v>626</v>
+      </c>
+      <c r="H255" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="I255" t="s">
+        <v>13</v>
+      </c>
+      <c r="J255" t="s">
+        <v>13</v>
+      </c>
+      <c r="K255" t="s">
+        <v>32</v>
+      </c>
+      <c r="L255" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected körnerStrack23 plot to raincloud
</commit_message>
<xml_diff>
--- a/raincloudQuartet_R/dataPbrPlotting.xlsx
+++ b/raincloudQuartet_R/dataPbrPlotting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Documents/GitHub/raincloudQuartet/raincloudQuartet_R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A4358D-3016-574A-A91D-36DB6B15F339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DD7BC9-B9BA-1B47-B5EB-E5D0E09B6919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{3C382137-58E4-F94B-B043-CDE1DB9A046F}"/>
   </bookViews>
@@ -2372,9 +2372,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2065784-6E08-3B41-935B-785814B2408A}">
   <dimension ref="A1:M255"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F256" sqref="F256"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="168" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2468,7 +2468,7 @@
         <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="21">

</xml_diff>